<commit_message>
This is my first project
</commit_message>
<xml_diff>
--- a/federo/src/test/resources/data/inputquotes.xlsx
+++ b/federo/src/test/resources/data/inputquotes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{89064579-12AF-418E-8833-DDDA1762BE62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{009DE711-2703-4E32-8684-01F5A43BBA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23280" windowHeight="13224" xr2:uid="{FE260C0C-045F-46DF-B1B9-3BBB1889DF7E}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23304" windowHeight="13224" xr2:uid="{FE260C0C-045F-46DF-B1B9-3BBB1889DF7E}"/>
   </bookViews>
   <sheets>
     <sheet name="quotes" sheetId="1" r:id="rId1"/>
@@ -16,21 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>subject</t>
   </si>
@@ -42,6 +33,21 @@
   </si>
   <si>
     <t>civil</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>qtyname</t>
+  </si>
+  <si>
+    <t>terabyte</t>
+  </si>
+  <si>
+    <t>list price</t>
   </si>
 </sst>
 </file>
@@ -394,32 +400,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8931AFA7-F676-4E7B-AA91-0A11BB38FCE3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>